<commit_message>
Updated eCPT Mapping sheet for RegulatoryAgencyIdentifierNumbers section.
</commit_message>
<xml_diff>
--- a/documents/sdr-release-v2.0.1/ddf-sdr-ri-usdm-cpt-mapping-sheet-v2.0.xlsx
+++ b/documents/sdr-release-v2.0.1/ddf-sdr-ri-usdm-cpt-mapping-sheet-v2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26707"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://transceleratebiopharma.sharepoint.com/harmonization/Digital Data Flow/Delivery Team/PUBLIC COLLABORATION/SDR Technical Documents/R2.0.1 Documentation/Set 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viswesh.mb\source\repos\Sprint 29\documents\sdr-release-v2.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4B83A43-34A4-4FF8-A144-BDE8FC4C23A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4096CAB1-7BE1-47CC-8FFD-8F5875F5C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{0B2AE8E1-EF95-4BFD-BBB7-E518A6021661}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{0B2AE8E1-EF95-4BFD-BBB7-E518A6021661}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer" sheetId="3" r:id="rId1"/>
@@ -62,8 +62,12 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={B03C6F38-B2F5-4180-A59D-69A8623956D2}</author>
-    <author>tc={6DDCAF13-3E1E-426F-A10B-3D7AD4D61D10}</author>
-    <author>tc={673C5124-C912-4066-BA62-32D49DEF50B7}</author>
+    <author>tc={C13D65B1-4591-4FE2-AAD8-60F281009780}</author>
+    <author>tc={E56E5E4F-CE40-4C5A-8C21-4F74A3879FF9}</author>
+    <author>tc={09D9882F-3874-48E9-A4ED-7927A51C33CE}</author>
+    <author>tc={2B0AEC58-DE36-4C65-B03C-F286826E5AC9}</author>
+    <author>tc={85092F17-0A58-4458-A4B1-24F300930709}</author>
+    <author>tc={E6C42F2B-C892-4499-85B9-D79FB3F2A458}</author>
   </authors>
   <commentList>
     <comment ref="J1" authorId="0" shapeId="0" xr:uid="{B03C6F38-B2F5-4180-A59D-69A8623956D2}">
@@ -74,20 +78,52 @@
     New column added with details on the default value of each variable in the SDR CPT response.</t>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{6DDCAF13-3E1E-426F-A10B-3D7AD4D61D10}">
+    <comment ref="I9" authorId="1" shapeId="0" xr:uid="{C13D65B1-4591-4FE2-AAD8-60F281009780}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands </t>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="2" shapeId="0" xr:uid="{E56E5E4F-CE40-4C5A-8C21-4F74A3879FF9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    USDM Field renamed from trialIntentType to trialIntentTypes.</t>
+    Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands</t>
       </text>
     </comment>
-    <comment ref="I9" authorId="2" shapeId="0" xr:uid="{673C5124-C912-4066-BA62-32D49DEF50B7}">
+    <comment ref="I11" authorId="3" shapeId="0" xr:uid="{09D9882F-3874-48E9-A4ED-7927A51C33CE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Logic description updated for objectives and endpoints to clarify that only the first primary or secondary objective will be considered if there are multiple.</t>
+    Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands</t>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="4" shapeId="0" xr:uid="{2B0AEC58-DE36-4C65-B03C-F286826E5AC9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands</t>
+      </text>
+    </comment>
+    <comment ref="I31" authorId="5" shapeId="0" xr:uid="{85092F17-0A58-4458-A4B1-24F300930709}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Refer attached screenshot for JSON sample for RegulatoryAgencyIdentifierNumbers</t>
+      </text>
+    </comment>
+    <comment ref="I32" authorId="6" shapeId="0" xr:uid="{E6C42F2B-C892-4499-85B9-D79FB3F2A458}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Refer attached screenshot for JSON sample for RegulatoryAgencyIdentifierNumbers</t>
       </text>
     </comment>
   </commentList>
@@ -95,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="322">
   <si>
     <t>Disclaimer</t>
   </si>
@@ -1663,12 +1699,21 @@
   <si>
     <t>Male</t>
   </si>
+  <si>
+    <t>RegulatoryAgencyIdentifierNumbers</t>
+  </si>
+  <si>
+    <t>CPT:RegulatoryAgencyIdentifierNumbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organisationIdentifierScheme | studyIdentifier </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1680,14 +1725,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1761,6 +1798,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1958,7 +2001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1967,15 +2010,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1985,10 +2028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2006,10 +2046,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2030,7 +2070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2048,22 +2088,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2095,6 +2135,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2316,19 +2368,19 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2385,13 +2437,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>8505825</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>4057650</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2430,16 +2482,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>8505825</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>11766</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4838700</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>4861111</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>540123</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2465,8 +2517,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="26708100" y="18630900"/>
-          <a:ext cx="4848225" cy="5000625"/>
+          <a:off x="26749001" y="2902323"/>
+          <a:ext cx="4849345" cy="5257800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2486,10 +2538,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B106B6C7-A51B-4459-A86F-6EE48FC68615}" name="Table2" displayName="Table2" ref="A1:J34" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
-  <autoFilter ref="A1:J34" xr:uid="{B106B6C7-A51B-4459-A86F-6EE48FC68615}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:I34">
-    <sortCondition ref="C2:C34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B106B6C7-A51B-4459-A86F-6EE48FC68615}" name="Table2" displayName="Table2" ref="A1:J35" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:J35" xr:uid="{B106B6C7-A51B-4459-A86F-6EE48FC68615}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:I35">
+    <sortCondition ref="C2:C35"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="3" xr3:uid="{242699DA-D4E7-449A-AC32-77A93CE9247D}" name="CPT ToC" dataDxfId="8"/>
@@ -2815,11 +2867,23 @@
   <threadedComment ref="J1" dT="2023-06-23T09:07:02.73" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{B03C6F38-B2F5-4180-A59D-69A8623956D2}">
     <text>New column added with details on the default value of each variable in the SDR CPT response.</text>
   </threadedComment>
-  <threadedComment ref="G6" dT="2023-06-23T09:07:54.21" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{6DDCAF13-3E1E-426F-A10B-3D7AD4D61D10}">
-    <text>USDM Field renamed from trialIntentType to trialIntentTypes.</text>
+  <threadedComment ref="I9" dT="2023-08-29T11:36:57.66" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{C13D65B1-4591-4FE2-AAD8-60F281009780}">
+    <text xml:space="preserve">Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands </text>
   </threadedComment>
-  <threadedComment ref="I9" dT="2023-06-23T09:14:41.89" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{673C5124-C912-4066-BA62-32D49DEF50B7}">
-    <text>Logic description updated for objectives and endpoints to clarify that only the first primary or secondary objective will be considered if there are multiple.</text>
+  <threadedComment ref="I10" dT="2023-08-29T11:37:02.20" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{E56E5E4F-CE40-4C5A-8C21-4F74A3879FF9}">
+    <text>Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands</text>
+  </threadedComment>
+  <threadedComment ref="I11" dT="2023-08-29T11:37:09.04" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{09D9882F-3874-48E9-A4ED-7927A51C33CE}">
+    <text>Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands</text>
+  </threadedComment>
+  <threadedComment ref="I12" dT="2023-08-29T11:37:13.20" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{2B0AEC58-DE36-4C65-B03C-F286826E5AC9}">
+    <text>Refer attached screenshot for JSON sample for ObectivesEndpointsAndEstimands</text>
+  </threadedComment>
+  <threadedComment ref="I31" dT="2023-08-29T11:38:50.17" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{85092F17-0A58-4458-A4B1-24F300930709}">
+    <text>Refer attached screenshot for JSON sample for RegulatoryAgencyIdentifierNumbers</text>
+  </threadedComment>
+  <threadedComment ref="I32" dT="2023-08-29T11:38:59.87" personId="{81C55B10-DBBD-4B16-AEBB-14CB34AF7DF4}" id="{E6C42F2B-C892-4499-85B9-D79FB3F2A458}">
+    <text>Refer attached screenshot for JSON sample for RegulatoryAgencyIdentifierNumbers</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2832,33 +2896,33 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="125.28515625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="125.28515625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.6">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30.95">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="77.45">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:1" ht="75.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="77.45">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2871,13 +2935,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E4FCAE-66AC-45EA-A062-1C146499097A}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -2887,75 +2951,75 @@
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="78" customWidth="1"/>
-    <col min="10" max="10" width="127.7109375" style="39" customWidth="1"/>
+    <col min="10" max="10" width="127.7109375" style="38" customWidth="1"/>
     <col min="11" max="11" width="79.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.5">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="39" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="29.1">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
@@ -2968,7 +3032,7 @@
       <c r="D3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2980,14 +3044,14 @@
       <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
@@ -3000,7 +3064,7 @@
       <c r="D4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -3012,14 +3076,14 @@
       <c r="H4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="40" t="s">
+      <c r="J4" s="39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="43.5">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
@@ -3032,7 +3096,7 @@
       <c r="D5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -3044,14 +3108,14 @@
       <c r="H5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.5">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -3064,7 +3128,7 @@
       <c r="D6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -3076,14 +3140,14 @@
       <c r="H6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>51</v>
       </c>
@@ -3093,10 +3157,10 @@
       <c r="C7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -3108,92 +3172,92 @@
       <c r="H7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>64</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="40"/>
-    </row>
-    <row r="9" spans="1:13" ht="45.75">
+      <c r="J8" s="39"/>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>68</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="39" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="43.5">
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -3205,59 +3269,59 @@
       <c r="H10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45.75">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>68</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="40" t="s">
+      <c r="J11" s="39" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45.75">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="10" t="s">
@@ -3269,14 +3333,14 @@
       <c r="H12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="40" t="s">
+      <c r="J12" s="39" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>84</v>
       </c>
@@ -3289,7 +3353,7 @@
       <c r="D13" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="10" t="s">
@@ -3301,14 +3365,14 @@
       <c r="H13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="40" t="s">
+      <c r="J13" s="39" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="87">
+    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>90</v>
       </c>
@@ -3321,7 +3385,7 @@
       <c r="D14" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="10" t="s">
@@ -3333,14 +3397,14 @@
       <c r="H14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="87">
+    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>90</v>
       </c>
@@ -3353,7 +3417,7 @@
       <c r="D15" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="10" t="s">
@@ -3365,14 +3429,14 @@
       <c r="H15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="26" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="144.94999999999999">
+    <row r="16" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>90</v>
       </c>
@@ -3385,7 +3449,7 @@
       <c r="D16" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -3397,411 +3461,411 @@
       <c r="H16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="43.5">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="10" t="s">
         <v>112</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="43.5">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="10" t="s">
         <v>117</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="43.5">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="10" t="s">
         <v>121</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="24" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="72.599999999999994">
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="10" t="s">
         <v>125</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="25" t="s">
+      <c r="I20" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="24" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="43.5">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>131</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="25" t="s">
+      <c r="I21" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="57.95">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>136</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="30" t="s">
         <v>138</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="J22" s="24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="57.95">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>143</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="30" t="s">
         <v>145</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="30" t="s">
         <v>151</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="J24" s="40" t="s">
+      <c r="J24" s="39" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="43.5">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>154</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="30" t="s">
         <v>156</v>
       </c>
       <c r="H25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="I25" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="J25" s="24" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="43.5">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>159</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="14" t="s">
         <v>161</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G26" s="32" t="s">
         <v>162</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="I26" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="24" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="29.1">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>165</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="30" t="s">
         <v>167</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="25" t="s">
+      <c r="I27" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="J27" s="24" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="43.5">
-      <c r="A28" s="22" t="s">
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="10" t="s">
         <v>172</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="25" t="s">
+      <c r="I28" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="24" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30.75">
-      <c r="A29" s="22" t="s">
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F29" s="10" t="s">
@@ -3813,178 +3877,208 @@
       <c r="H29" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="25" t="s">
+      <c r="I29" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="J29" s="40" t="s">
+      <c r="J29" s="39" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30.75">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>27</v>
+      <c r="C30" s="49" t="s">
+        <v>319</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>320</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="J30" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="K30" s="43"/>
-    </row>
-    <row r="31" spans="1:11" ht="30.75">
-      <c r="A31" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="H30" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="39"/>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>134</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>185</v>
+      <c r="C31" s="27" t="s">
+        <v>180</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>22</v>
+        <v>181</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>187</v>
+        <v>28</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>182</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="I31" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="J31" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="K31" s="43"/>
-    </row>
-    <row r="32" spans="1:11" ht="45.75">
-      <c r="A32" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="K31" s="42"/>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>148</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E32" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="J32" s="25" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="29.1">
-      <c r="A33" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I32" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="J32" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="K32" s="42"/>
+    </row>
+    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="28" t="s">
-        <v>194</v>
+      <c r="C33" s="27" t="s">
+        <v>189</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="E33" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>196</v>
+      <c r="G33" s="30" t="s">
+        <v>191</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J33" s="25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="29.1">
-      <c r="A34" s="18" t="s">
+      <c r="I33" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="J33" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="J34" s="24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E35" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H35" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="I34" s="25" t="s">
+      <c r="I35" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="J34" s="25" t="s">
+      <c r="J35" s="24" t="s">
         <v>204</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K31:K32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4004,7 +4098,7 @@
       <selection activeCell="D4" sqref="D4:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="34.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -4019,22 +4113,22 @@
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>206</v>
       </c>
@@ -4061,7 +4155,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>210</v>
       </c>
@@ -4083,7 +4177,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>216</v>
       </c>
@@ -4107,7 +4201,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>223</v>
       </c>
@@ -4131,7 +4225,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>230</v>
       </c>
@@ -4155,7 +4249,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>237</v>
       </c>
@@ -4179,7 +4273,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>244</v>
       </c>
@@ -4197,7 +4291,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>248</v>
       </c>
@@ -4215,7 +4309,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1">
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>251</v>
       </c>
@@ -4229,7 +4323,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1">
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>254</v>
       </c>
@@ -4243,7 +4337,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>258</v>
       </c>
@@ -4257,7 +4351,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>261</v>
       </c>
@@ -4271,7 +4365,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>264</v>
       </c>
@@ -4285,7 +4379,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>268</v>
       </c>
@@ -4299,25 +4393,25 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="12" customHeight="1">
-      <c r="A17" s="48" t="s">
+    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
         <v>272</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>206</v>
       </c>
@@ -4343,7 +4437,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>274</v>
       </c>
@@ -4363,7 +4457,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>279</v>
       </c>
@@ -4381,7 +4475,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>283</v>
       </c>
@@ -4393,7 +4487,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>286</v>
       </c>
@@ -4405,7 +4499,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>289</v>
       </c>
@@ -4415,7 +4509,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>291</v>
       </c>
@@ -4427,7 +4521,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>294</v>
       </c>
@@ -4437,7 +4531,7 @@
       <c r="C25" s="5"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="5"/>
@@ -4445,7 +4539,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>297</v>
       </c>
@@ -4457,7 +4551,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>300</v>
       </c>
@@ -4469,7 +4563,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>303</v>
       </c>
@@ -4481,7 +4575,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>306</v>
       </c>
@@ -4493,15 +4587,15 @@
         <v>308</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="48" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
         <v>309</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>206</v>
       </c>
@@ -4515,7 +4609,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>310</v>
       </c>
@@ -4527,7 +4621,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>313</v>
       </c>
@@ -4541,7 +4635,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>316</v>
       </c>
@@ -4568,15 +4662,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F70ACD1D198BA4A93FC70EBD4D0E4F5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18b475abf70eecdc601daa3e136f5dd8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ff55c19-750b-4d57-96fc-c7d80b080a4b" xmlns:ns3="a951cd76-9ac8-4a77-9c78-24aa33457680" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74bfc7bfa49a56144affddbcba5bb63a" ns2:_="" ns3:_="">
     <xsd:import namespace="9ff55c19-750b-4d57-96fc-c7d80b080a4b"/>
@@ -4795,6 +4880,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4814,15 +4908,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ECA9E88-1B99-4474-8978-A91F02949421}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6F278E2-9CE3-4EF4-840E-7AB4B281D7EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ff55c19-750b-4d57-96fc-c7d80b080a4b"/>
+    <ds:schemaRef ds:uri="a951cd76-9ac8-4a77-9c78-24aa33457680"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6F278E2-9CE3-4EF4-840E-7AB4B281D7EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ECA9E88-1B99-4474-8978-A91F02949421}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6207C920-2DE1-49C4-BD21-29E62428C2D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6207C920-2DE1-49C4-BD21-29E62428C2D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9ff55c19-750b-4d57-96fc-c7d80b080a4b"/>
+    <ds:schemaRef ds:uri="a951cd76-9ac8-4a77-9c78-24aa33457680"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>